<commit_message>
XML Update 5 - FIB, MCQ, FIB/MCQ Complete
</commit_message>
<xml_diff>
--- a/Copy of for Tutelages_Error_Tables.xlsx
+++ b/Copy of for Tutelages_Error_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Apple/Myscripts/Javascript/googleT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1955660D-96A3-FC46-95B1-C0B8C88D85F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F3D58C-2E14-0D41-9CEB-A3D611E86C9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="4" xr2:uid="{ABB644EC-2FF6-4E8E-A5BE-C1ADA6D6C56E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="5" xr2:uid="{ABB644EC-2FF6-4E8E-A5BE-C1ADA6D6C56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6 (2)" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet6 (3)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="46">
   <si>
     <t>A</t>
   </si>
@@ -163,6 +165,15 @@
   </si>
   <si>
     <t>A, B</t>
+  </si>
+  <si>
+    <t>FIB/MCQ</t>
+  </si>
+  <si>
+    <t>FIBTest</t>
+  </si>
+  <si>
+    <t>aaaMCQTest</t>
   </si>
 </sst>
 </file>
@@ -769,7 +780,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1023,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1068,6 +1079,254 @@
       </c>
       <c r="B4" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F203E4E9-9FED-DB43-B3DD-AE8B62DB7CB3}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA70F8-8B85-C449-ACCF-CBC42407937C}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
XML Update 5 - FIB, MCQ, FIB/MCQ, SLOT Complete
</commit_message>
<xml_diff>
--- a/Copy of for Tutelages_Error_Tables.xlsx
+++ b/Copy of for Tutelages_Error_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Apple/Myscripts/Javascript/googleT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F3D58C-2E14-0D41-9CEB-A3D611E86C9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1FF070-E680-E349-A508-FA6E7786A3AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="5" xr2:uid="{ABB644EC-2FF6-4E8E-A5BE-C1ADA6D6C56E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="57">
   <si>
     <t>A</t>
   </si>
@@ -173,7 +173,40 @@
     <t>FIBTest</t>
   </si>
   <si>
-    <t>aaaMCQTest</t>
+    <t>Slot1L: Slot3R;Slot2L: Slot1R;Slot3L: Slot4R;Slot4L: Slot 2R</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Slot1L ≠ Slot3R</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>Slot2L ≠ Slot1R</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>Slot3L ≠ Slot4R</t>
+  </si>
+  <si>
+    <t>FD3</t>
+  </si>
+  <si>
+    <t>Slot4L ≠ Slot2R</t>
+  </si>
+  <si>
+    <t>FD4</t>
+  </si>
+  <si>
+    <t>SLOT</t>
+  </si>
+  <si>
+    <t>SLOT Test</t>
   </si>
 </sst>
 </file>
@@ -209,9 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,7 +1182,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F203E4E9-9FED-DB43-B3DD-AE8B62DB7CB3}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -1183,7 +1220,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1">
         <v>4</v>
@@ -1202,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1218,48 +1255,89 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>